<commit_message>
test with real data
</commit_message>
<xml_diff>
--- a/drying1.xlsx
+++ b/drying1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitsy\OneDrive - Hanzehogeschool Groningen\master SSE\ESKA\Drying-process-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{67C6D4AC-CE87-45BD-90D3-D4F888DC1BB3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F940C34A-EBF0-4099-A028-1AE09AE8078A}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{67C6D4AC-CE87-45BD-90D3-D4F888DC1BB3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2F8310D6-2CEA-47C2-8F65-814133DC4ED2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{21342FDE-E0F2-44F7-A2C0-BB21EE6451C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{21342FDE-E0F2-44F7-A2C0-BB21EE6451C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,12 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Sensor</t>
   </si>
   <si>
     <t>Weigh (g)</t>
+  </si>
+  <si>
+    <t>Dry weigh</t>
   </si>
 </sst>
 </file>
@@ -2628,7 +2632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302CFEF7-F961-44D8-80C9-70FA3E68B5DA}">
   <dimension ref="E2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+    <sheetView topLeftCell="C2" workbookViewId="0">
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
@@ -2817,6 +2821,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F237DF5D-3879-4E6B-8809-0A364B9BE692}">
+  <dimension ref="D2:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="G3">
+        <v>2.46</v>
+      </c>
+      <c r="H3">
+        <v>100.9</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="H4">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>2.56</v>
+      </c>
+      <c r="H5">
+        <v>96.6</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>2.73</v>
+      </c>
+      <c r="H6">
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>2.92</v>
+      </c>
+      <c r="H7">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>3.05</v>
+      </c>
+      <c r="H8">
+        <v>80.3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>3.32</v>
+      </c>
+      <c r="H9">
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>3.54</v>
+      </c>
+      <c r="H10">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>3.7</v>
+      </c>
+      <c r="H11">
+        <v>65.2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>3.91</v>
+      </c>
+      <c r="H12">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>4.2</v>
+      </c>
+      <c r="H13">
+        <v>54.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73613A8D-0E6A-4BD1-9CFE-29909F153C90}">
   <dimension ref="E2:F23"/>
   <sheetViews>
@@ -3009,21 +3124,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006AAA3DE7CEDA749B21B395C352DDF75" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="a95fdc84068296bbbf8f2f90f99e9606">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="911050ce-e905-4290-8ac0-89b6f4c0a8b2" xmlns:ns4="77f72f0b-ec28-4622-9e0a-e58463c12532" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="39ee3fba80951e449748d94f9f67cbe6" ns3:_="" ns4:_="">
     <xsd:import namespace="911050ce-e905-4290-8ac0-89b6f4c0a8b2"/>
@@ -3246,32 +3346,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{807CA3D5-20E2-472A-9F95-AA64F0ADB6F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="77f72f0b-ec28-4622-9e0a-e58463c12532"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="911050ce-e905-4290-8ac0-89b6f4c0a8b2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{833A6394-5C96-4E9E-BC24-DA4A63D501D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EFC103F-7A00-4BDB-AA6C-A9A08BC9C00B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3288,4 +3378,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{833A6394-5C96-4E9E-BC24-DA4A63D501D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{807CA3D5-20E2-472A-9F95-AA64F0ADB6F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="77f72f0b-ec28-4622-9e0a-e58463c12532"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="911050ce-e905-4290-8ac0-89b6f4c0a8b2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
open new data + convert epoch date format
</commit_message>
<xml_diff>
--- a/drying1.xlsx
+++ b/drying1.xlsx
@@ -3347,18 +3347,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3381,26 +3381,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{807CA3D5-20E2-472A-9F95-AA64F0ADB6F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="911050ce-e905-4290-8ac0-89b6f4c0a8b2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="77f72f0b-ec28-4622-9e0a-e58463c12532"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{833A6394-5C96-4E9E-BC24-DA4A63D501D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{807CA3D5-20E2-472A-9F95-AA64F0ADB6F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="77f72f0b-ec28-4622-9e0a-e58463c12532"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="911050ce-e905-4290-8ac0-89b6f4c0a8b2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>